<commit_message>
test coverage has been rised
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\176619\se-lab-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E154D527-4E2D-468B-832F-41847862FEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5019557-4C95-4BA0-9370-164A864FB08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4E0E450-1A81-4C66-9206-C949033C9C0A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="31">
   <si>
     <t>Tesztelt követelmény</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Nem működik a torpedo SINGLE methodja, ha 0 van mindkét Storeban, tehát nem fog tüzelni</t>
+  </si>
+  <si>
+    <t>SINGLE módban először a Primaryből bayből tüzelne, de hibás lesz a lövés</t>
   </si>
 </sst>
 </file>
@@ -476,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5913BA62-234E-41B5-A8CB-52E6D7ABEFEB}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,6 +811,38 @@
         <v>7</v>
       </c>
     </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>